<commit_message>
checkbox auto nuevo y subir factura
</commit_message>
<xml_diff>
--- a/datos/datos_extraidos.xlsx
+++ b/datos/datos_extraidos.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Datos Extraídos" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,7 +450,7 @@
     <col width="21" customWidth="1" min="14" max="14"/>
     <col width="17" customWidth="1" min="15" max="15"/>
     <col width="20" customWidth="1" min="16" max="16"/>
-    <col width="10" customWidth="1" min="17" max="17"/>
+    <col width="11" customWidth="1" min="17" max="17"/>
     <col width="12" customWidth="1" min="18" max="18"/>
   </cols>
   <sheetData>
@@ -619,20 +619,112 @@
       </c>
       <c r="O2" s="2" t="inlineStr">
         <is>
-          <t>Antioquia</t>
+          <t>Risaralda</t>
         </is>
       </c>
       <c r="P2" s="2" t="inlineStr">
         <is>
-          <t>Girardota</t>
+          <t>Dosquebradas</t>
         </is>
       </c>
       <c r="Q2" s="2" t="inlineStr">
         <is>
-          <t>FEMENINO</t>
+          <t>MASCULINO</t>
         </is>
       </c>
       <c r="R2" s="2" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>1.087.985.773</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>CARLOS ALBERTO</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>LADINO OCAMPO</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>17-JUN-2004</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>11-JUL-2022 DOSQUEBRADAS</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>carlosladino.iearm6@gmail.com</t>
+        </is>
+      </c>
+      <c r="G3" s="2" t="inlineStr">
+        <is>
+          <t>AUTOMOVIL</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="inlineStr">
+        <is>
+          <t>GTP296</t>
+        </is>
+      </c>
+      <c r="I3" s="2" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="J3" s="2" t="inlineStr">
+        <is>
+          <t>PARTICULAR</t>
+        </is>
+      </c>
+      <c r="K3" s="2" t="inlineStr">
+        <is>
+          <t>KIA</t>
+        </is>
+      </c>
+      <c r="L3" s="2" t="inlineStr">
+        <is>
+          <t>PICANTO</t>
+        </is>
+      </c>
+      <c r="M3" s="2" t="inlineStr">
+        <is>
+          <t>1.248</t>
+        </is>
+      </c>
+      <c r="N3" s="2" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="O3" s="2" t="inlineStr">
+        <is>
+          <t>Risaralda</t>
+        </is>
+      </c>
+      <c r="P3" s="2" t="inlineStr">
+        <is>
+          <t>Pereira</t>
+        </is>
+      </c>
+      <c r="Q3" s="2" t="inlineStr">
+        <is>
+          <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="R3" s="2" t="inlineStr">
         <is>
           <t>DAVIVIENDA</t>
         </is>

</xml_diff>